<commit_message>
added product details data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginTestData.xlsx
+++ b/src/test/resources/LoginTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdroh\IdeaProjects\SauceDemoTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81653443-3ED5-47B6-B0EF-01D3EAA27FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C839C1-81A4-4301-AB3E-98D1DF818E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -61,15 +62,83 @@
   </si>
   <si>
     <t>Url contains inventory.html</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>Product Price</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt</t>
+  </si>
+  <si>
+    <t>carry.allTheThings() with the sleek, streamlined Sly Pack that melds uncompromising style with unequaled laptop and tablet protection.</t>
+  </si>
+  <si>
+    <t>$29.99</t>
+  </si>
+  <si>
+    <t>A red light isn't the desired state in testing but it sure helps when riding your bike at night. Water-resistant with 3 lighting modes, 1 AAA battery included.</t>
+  </si>
+  <si>
+    <t>$9.99</t>
+  </si>
+  <si>
+    <t>Get your testing superhero on with the Sauce Labs bolt T-shirt. From American Apparel, 100% ringspun combed cotton, heather gray with red bolt.</t>
+  </si>
+  <si>
+    <t>$15.99</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>It's not every day that you come across a midweight quarter-zip fleece jacket capable of handling everything from a relaxing day outdoors to a busy day at the office.</t>
+  </si>
+  <si>
+    <t>$49.99</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Rib snap infant onesie for the junior automation engineer in development. Reinforced 3-snap bottom closure, two-needle hemmed sleeved and bottom won't unravel.</t>
+  </si>
+  <si>
+    <t>$7.99</t>
+  </si>
+  <si>
+    <t>Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>This classic Sauce Labs t-shirt is perfect to wear when cozying up to your keyboard to automate a few tests. Super-soft and comfy ringspun combed cotton.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -96,8 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -466,4 +536,101 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EADE38C-DE67-495F-8150-79547D21A72F}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="138.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>